<commit_message>
Update RedDot System and Add ModelManager
</commit_message>
<xml_diff>
--- a/ExcelData/__tables__.xlsx
+++ b/ExcelData/__tables__.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>##var</t>
   </si>
@@ -116,7 +116,16 @@
     <t>DateCardsDB</t>
   </si>
   <si>
-    <t>schedule/datedata.xlsx</t>
+    <t>schedule/dateData.xlsx</t>
+  </si>
+  <si>
+    <t>MessageReaderDB</t>
+  </si>
+  <si>
+    <t>MessageDB</t>
+  </si>
+  <si>
+    <t>phone/phoneMessageData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1058,18 +1067,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="4"/>
   <cols>
     <col min="2" max="2" width="20.3796296296296" customWidth="1"/>
     <col min="3" max="3" width="15.6296296296296" customWidth="1"/>
     <col min="4" max="4" width="32.3796296296296" customWidth="1"/>
-    <col min="5" max="5" width="24.3796296296296" customWidth="1"/>
+    <col min="5" max="5" width="31.3333333333333" customWidth="1"/>
     <col min="6" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1175,6 +1184,20 @@
       </c>
       <c r="E4" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add message and dialog xls files
Signed-off-by: SkySakura <1693385825@qq.com>
</commit_message>
<xml_diff>
--- a/ExcelData/__tables__.xlsx
+++ b/ExcelData/__tables__.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>##var</t>
   </si>
@@ -119,13 +119,22 @@
     <t>schedule/dateData.xlsx</t>
   </si>
   <si>
-    <t>MessageReaderDB</t>
+    <t>phone.MessageReaderDB</t>
   </si>
   <si>
     <t>MessageDB</t>
   </si>
   <si>
     <t>phone/phoneMessageData.xlsx</t>
+  </si>
+  <si>
+    <t>dialog.DialogReaderDB</t>
+  </si>
+  <si>
+    <t>DiglogDB</t>
+  </si>
+  <si>
+    <t>dialog/mainDialogData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1067,13 +1076,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="5"/>
   <cols>
     <col min="2" max="2" width="20.3796296296296" customWidth="1"/>
     <col min="3" max="3" width="15.6296296296296" customWidth="1"/>
@@ -1200,6 +1209,20 @@
         <v>32</v>
       </c>
     </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Add the new dialog system.
Signed-off-by: SkySakura <1693385825@qq.com>
</commit_message>
<xml_diff>
--- a/ExcelData/__tables__.xlsx
+++ b/ExcelData/__tables__.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
@@ -131,7 +131,7 @@
     <t>dialog.DialogReaderDB</t>
   </si>
   <si>
-    <t>DiglogDB</t>
+    <t>DialogDB</t>
   </si>
   <si>
     <t>dialog/mainDialogData.xlsx</t>
@@ -816,6 +816,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1079,7 +1086,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="5"/>

</xml_diff>